<commit_message>
Added litter numbers version
</commit_message>
<xml_diff>
--- a/Voles.xlsx
+++ b/Voles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynn\Documents\GitHub\ST542-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBFFC50-685E-4746-BE1A-40CC9827B94B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8FB828-59C5-4457-B60A-B59B62192A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{030A0D1B-C587-41FF-A484-1168540D0085}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{030A0D1B-C587-41FF-A484-1168540D0085}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2162,7 +2162,7 @@
   <dimension ref="A1:T248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>